<commit_message>
added pul-ups for encoder A,B,Switch, board rerouted, euricircuits pass and new auto quotation
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\n-blocks\upa-dip\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7D0F14D-7485-4254-AC00-9201EF3EDE1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC30C2E5-C6F3-493F-8DDA-CED34E6F0589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29010" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseList" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <t>UPA-DIP-V2</t>
   </si>
   <si>
-    <t>15:31</t>
+    <t>21:45</t>
   </si>
   <si>
     <t>40</t>
@@ -80,10 +80,10 @@
     <t>C2, C4</t>
   </si>
   <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>R1</t>
+    <t>J2, J3</t>
+  </si>
+  <si>
+    <t>R1, R3, R4, R5</t>
   </si>
   <si>
     <t>R2</t>
@@ -95,10 +95,10 @@
     <t>B1</t>
   </si>
   <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>LCD1</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J4</t>
   </si>
   <si>
     <t>U1</t>
@@ -131,12 +131,12 @@
     <t>N-GMS-NO-PINS</t>
   </si>
   <si>
+    <t>LCD MODULE SIL</t>
+  </si>
+  <si>
     <t>HEADER_5</t>
   </si>
   <si>
-    <t>LCD MODULE SIL</t>
-  </si>
-  <si>
     <t>ATmega328PU</t>
   </si>
   <si>
@@ -158,10 +158,10 @@
     <t>BUTTON_6X6mm</t>
   </si>
   <si>
+    <t>1X14-FEMALE</t>
+  </si>
+  <si>
     <t>1X05</t>
-  </si>
-  <si>
-    <t>1X14-FEMALE</t>
   </si>
   <si>
     <t>DIL28-300wSOCKET</t>
@@ -1119,7 +1119,7 @@
         <v>65</v>
       </c>
       <c r="J2" s="10">
-        <v>105761</v>
+        <v>101930</v>
       </c>
       <c r="K2" s="46" t="s">
         <v>68</v>
@@ -1138,11 +1138,11 @@
         <v>10</v>
       </c>
       <c r="P2" s="30">
-        <v>9.1770000000000004E-2</v>
+        <v>9.0160000000000004E-2</v>
       </c>
       <c r="Q2" s="30">
         <f>P2*O2</f>
-        <v>0.91770000000000007</v>
+        <v>0.90160000000000007</v>
       </c>
       <c r="R2" s="48">
         <f>ROW(R2) - ROW($A$1)</f>
@@ -1225,7 +1225,7 @@
         <v>65</v>
       </c>
       <c r="J4" s="10">
-        <v>0</v>
+        <v>2985</v>
       </c>
       <c r="K4" s="46" t="s">
         <v>69</v>
@@ -1244,11 +1244,11 @@
         <v>10</v>
       </c>
       <c r="P4" s="30">
-        <v>0.50563999999999998</v>
+        <v>0.49679000000000001</v>
       </c>
       <c r="Q4" s="30">
         <f>P4*O4</f>
-        <v>5.0564</v>
+        <v>4.9679000000000002</v>
       </c>
       <c r="R4" s="48">
         <f>ROW(R4) - ROW($A$1)</f>
@@ -1285,7 +1285,7 @@
         <v>65</v>
       </c>
       <c r="J5" s="10">
-        <v>6960</v>
+        <v>6950</v>
       </c>
       <c r="K5" s="46" t="s">
         <v>70</v>
@@ -1294,21 +1294,21 @@
         <v>1</v>
       </c>
       <c r="M5" s="10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N5" s="44">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="O5" s="47">
         <f t="shared" ref="O5" si="4">ROUNDUP(N5*L5,0)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P5" s="30">
-        <v>9.1770000000000004E-2</v>
+        <v>9.0160000000000004E-2</v>
       </c>
       <c r="Q5" s="30">
         <f t="shared" ref="Q5" si="5">P5*O5</f>
-        <v>0.45885000000000004</v>
+        <v>1.8032000000000001</v>
       </c>
       <c r="R5" s="48">
         <f t="shared" si="3"/>
@@ -1410,11 +1410,11 @@
         <v>5</v>
       </c>
       <c r="P7" s="30">
-        <v>0.68825999999999998</v>
+        <v>0.67620999999999998</v>
       </c>
       <c r="Q7" s="30">
         <f t="shared" ref="Q7:Q9" si="7">P7*O7</f>
-        <v>3.4413</v>
+        <v>3.3810500000000001</v>
       </c>
       <c r="R7" s="48">
         <f t="shared" si="3"/>
@@ -1475,7 +1475,9 @@
       <c r="D9" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
       <c r="H9" s="52"/>
@@ -1515,9 +1517,7 @@
       <c r="D10" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="E10" s="9"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
       <c r="H10" s="52"/>
@@ -1667,7 +1667,7 @@
       <c r="J14" s="14"/>
       <c r="K14" s="34">
         <f ca="1">NOW()</f>
-        <v>43975.646852430553</v>
+        <v>43981.90647627315</v>
       </c>
       <c r="L14" s="40"/>
       <c r="M14" s="15"/>
@@ -1678,11 +1678,11 @@
       </c>
       <c r="Q14" s="36">
         <f>SUM(Q2:Q12)</f>
-        <v>9.87425</v>
+        <v>11.053750000000001</v>
       </c>
       <c r="R14" s="50">
         <f>Q14/N15</f>
-        <v>0.24685625</v>
+        <v>0.27634375</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>